<commit_message>
Update Python script that converts excel to jsonld
</commit_message>
<xml_diff>
--- a/Metadata_Experiment_Objects.xlsx
+++ b/Metadata_Experiment_Objects.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12045" firstSheet="19" activeTab="21"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12045"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment" sheetId="11" r:id="rId1"/>
@@ -1260,14 +1260,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2779,7 +2779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BA1" workbookViewId="0">
+    <sheetView topLeftCell="BA1" workbookViewId="0">
       <selection activeCell="BE9" sqref="BE9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update metadata files and add RDFLib script
</commit_message>
<xml_diff>
--- a/Metadata_Experiment_Objects.xlsx
+++ b/Metadata_Experiment_Objects.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12045" firstSheet="13" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12045"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment" sheetId="11" r:id="rId1"/>
@@ -1260,7 +1260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -2547,7 +2547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>

</xml_diff>